<commit_message>
Update Command Line portion of FIS Prework.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -10,7 +10,7 @@
     <sheet name="FIS PreWork" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DateList">'FIS PreWork'!$G$5:$G$39</definedName>
+    <definedName name="DateList">'FIS PreWork'!$E$5:$E$42</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Course / Subject</t>
   </si>
@@ -52,15 +52,6 @@
   </si>
   <si>
     <t>Learn the Cmd Line the Hard Way</t>
-  </si>
-  <si>
-    <t>Time Est.</t>
-  </si>
-  <si>
-    <t>Time Act.</t>
-  </si>
-  <si>
-    <t>Cmd Line Basics</t>
   </si>
   <si>
     <t>Learn SQL the Hard Way</t>
@@ -184,9 +175,6 @@
 Practices</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Getting Started with Rails</t>
   </si>
   <si>
@@ -194,16 +182,25 @@
   </si>
   <si>
     <t>Command Line Tutorial</t>
+  </si>
+  <si>
+    <t>Getting Started with the Console</t>
+  </si>
+  <si>
+    <t>Environment and Redirection</t>
+  </si>
+  <si>
+    <t>Console Foundations</t>
+  </si>
+  <si>
+    <t>Command Line Basics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +229,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -753,11 +758,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -876,60 +885,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -945,6 +900,42 @@
     <xf numFmtId="14" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -978,44 +969,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1316,13 +1275,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G42"/>
+  <dimension ref="B1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1330,25 +1289,22 @@
     <col min="1" max="1" width="1.5" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.83203125" style="1"/>
     <col min="4" max="4" width="32.1640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="40" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="18.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:7" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="74" t="s">
+    <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="76"/>
-    </row>
-    <row r="3" spans="2:7" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
-    <row r="4" spans="2:7" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
+    <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B4" s="39" t="s">
         <v>6</v>
       </c>
@@ -1358,587 +1314,401 @@
       <c r="D4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="41" t="s">
+      <c r="E4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="77" t="s">
+    </row>
+    <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="50" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="42">
-        <v>1.5</v>
-      </c>
-      <c r="F5" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="E5" s="10">
         <v>41368</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+    <row r="6" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="43">
-        <v>2</v>
-      </c>
-      <c r="F6" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="12">
+      <c r="E6" s="12">
         <v>41368</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="78"/>
-      <c r="C7" s="79"/>
+    <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="F7" s="44">
-        <v>1.5</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="E7" s="10">
         <v>41373</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="78"/>
-      <c r="C8" s="80" t="s">
+    <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B8" s="49"/>
+      <c r="C8" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="42">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B9" s="49"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B10" s="49"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B11" s="49"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B12" s="49"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="12">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B13" s="49"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="41"/>
+    </row>
+    <row r="14" spans="2:5" ht="27" thickTop="1" thickBot="1">
+      <c r="B14" s="49"/>
+      <c r="C14" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="10">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B15" s="49"/>
+      <c r="C15" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="42">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B16" s="49"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="12">
+        <v>41422</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B17" s="49"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="41">
+        <v>41422</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B18" s="49"/>
+      <c r="C18" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B19" s="49"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B20" s="49"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B21" s="49"/>
+      <c r="C21" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="10">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="12">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="10">
+        <v>41427</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B26" s="5"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B27" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="60">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B9" s="78"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="12">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B10" s="78"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="46">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="59">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="27" thickTop="1" thickBot="1">
-      <c r="B11" s="78"/>
-      <c r="C11" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="44">
-        <v>4</v>
-      </c>
-      <c r="F11" s="44">
-        <v>4</v>
-      </c>
-      <c r="G11" s="10">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B12" s="78"/>
-      <c r="C12" s="80" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="45">
-        <v>2</v>
-      </c>
-      <c r="F12" s="45">
-        <v>2</v>
-      </c>
-      <c r="G12" s="60">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B13" s="78"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="43">
-        <v>6</v>
-      </c>
-      <c r="F13" s="43">
-        <v>4</v>
-      </c>
-      <c r="G13" s="12">
-        <v>41422</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B14" s="78"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="46">
-        <v>6</v>
-      </c>
-      <c r="F14" s="46">
-        <v>5</v>
-      </c>
-      <c r="G14" s="59">
-        <v>41422</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B15" s="78"/>
-      <c r="C15" s="83" t="s">
+      <c r="D27" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="48">
-        <v>10</v>
-      </c>
-      <c r="F15" s="48">
-        <v>4</v>
-      </c>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B16" s="78"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="43">
-        <v>6</v>
-      </c>
-      <c r="F16" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="2:7" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B17" s="78"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="47">
-        <v>4</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B18" s="78"/>
-      <c r="C18" s="79" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="44">
-        <v>1</v>
-      </c>
-      <c r="F18" s="44">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="10">
+      <c r="E27" s="43">
         <v>41423</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B19" s="78"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="43">
-        <v>4</v>
-      </c>
-      <c r="F19" s="43">
-        <v>2</v>
-      </c>
-      <c r="G19" s="12">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B20" s="78"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="43">
-        <v>3</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B21" s="78"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="43">
-        <v>6</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B22" s="78"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="44">
-        <v>1</v>
-      </c>
-      <c r="F22" s="44">
-        <v>1</v>
-      </c>
-      <c r="G22" s="10">
+    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B28" s="57"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="44">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B29" s="57"/>
+      <c r="C29" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="28">
+        <v>41425</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B30" s="57"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="27"/>
+    </row>
+    <row r="31" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B31" s="57"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B32" s="57"/>
+      <c r="C32" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="25"/>
+    </row>
+    <row r="33" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B33" s="57"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="29">
         <v>41427</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="3.75" customHeight="1">
-      <c r="B23" s="5"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B24" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="50">
-        <v>1</v>
-      </c>
-      <c r="F24" s="50">
-        <v>1</v>
-      </c>
-      <c r="G24" s="61">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B25" s="63"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="51">
-        <v>4</v>
-      </c>
-      <c r="F25" s="51">
-        <v>1.5</v>
-      </c>
-      <c r="G25" s="62">
-        <v>41424</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B26" s="63"/>
-      <c r="C26" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="52">
-        <v>6</v>
-      </c>
-      <c r="F26" s="52">
-        <v>4</v>
-      </c>
-      <c r="G26" s="28">
-        <v>41425</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B27" s="63"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="53">
-        <v>6</v>
-      </c>
-      <c r="F27" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="27"/>
-    </row>
-    <row r="28" spans="2:7" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B28" s="63"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="51">
-        <v>6</v>
-      </c>
-      <c r="F28" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="23"/>
-    </row>
-    <row r="29" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B29" s="63"/>
-      <c r="C29" s="66" t="s">
+    <row r="34" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B34" s="57"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="E34" s="23"/>
+    </row>
+    <row r="35" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B35" s="57"/>
+      <c r="C35" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="52">
-        <v>10</v>
-      </c>
-      <c r="F29" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="25"/>
-    </row>
-    <row r="30" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B30" s="63"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="26" t="s">
+      <c r="D35" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="28"/>
+    </row>
+    <row r="36" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B36" s="57"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="43"/>
+    </row>
+    <row r="37" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B37" s="57"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="53">
-        <v>10</v>
-      </c>
-      <c r="F30" s="53">
-        <v>6</v>
-      </c>
-      <c r="G30" s="29">
-        <v>41427</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B31" s="63"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="22" t="s">
+      <c r="E37" s="29"/>
+    </row>
+    <row r="38" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B38" s="57"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="51">
-        <v>6</v>
-      </c>
-      <c r="F31" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" s="23"/>
-    </row>
-    <row r="32" spans="2:7" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B32" s="63"/>
-      <c r="C32" s="66" t="s">
+      <c r="E38" s="31"/>
+    </row>
+    <row r="39" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B39" s="6"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="2:5" ht="26.25" customHeight="1">
+      <c r="B40" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" s="52">
-        <v>2</v>
-      </c>
-      <c r="F32" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="28"/>
-    </row>
-    <row r="33" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B33" s="63"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E33" s="50">
-        <v>4</v>
-      </c>
-      <c r="F33" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" s="61"/>
-    </row>
-    <row r="34" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B34" s="63"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="26" t="s">
+      <c r="D40" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="53">
-        <v>4</v>
-      </c>
-      <c r="F34" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="G34" s="29"/>
-    </row>
-    <row r="35" spans="2:7" ht="18.75" customHeight="1">
-      <c r="B35" s="63"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="30" t="s">
+      <c r="E40" s="34"/>
+    </row>
+    <row r="41" spans="2:5" ht="26.25" customHeight="1" thickBot="1">
+      <c r="B41" s="64"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="54">
-        <v>12</v>
-      </c>
-      <c r="F35" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="G35" s="31"/>
-    </row>
-    <row r="36" spans="2:7" ht="3.75" customHeight="1">
-      <c r="B36" s="6"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="2:7" ht="26.25" customHeight="1">
-      <c r="B37" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="72" t="s">
+      <c r="E41" s="36"/>
+    </row>
+    <row r="42" spans="2:5" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B42" s="65"/>
+      <c r="C42" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="55">
-        <v>5</v>
-      </c>
-      <c r="F37" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="G37" s="34"/>
-    </row>
-    <row r="38" spans="2:7" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B38" s="70"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="56">
-        <v>5</v>
-      </c>
-      <c r="F38" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="G38" s="36"/>
-    </row>
-    <row r="39" spans="2:7" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B39" s="71"/>
-      <c r="C39" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="57">
-        <v>5</v>
-      </c>
-      <c r="F39" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="G39" s="38"/>
-    </row>
-    <row r="40" spans="2:7" ht="18.75" customHeight="1" thickTop="1"/>
-    <row r="41" spans="2:7" ht="18.75" customHeight="1">
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="2:7" ht="18.75" customHeight="1">
-      <c r="G42" s="8"/>
+      <c r="E42" s="38"/>
+    </row>
+    <row r="43" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
+    <row r="44" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E45" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B5:B22"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B27:B38"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B5:B25"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C8:C13"/>
     <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="B24:B35"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2:G2" r:id="rId1" display="The Flatiron School Prework"/>
+    <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update FIS Prework with SQL content.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="0" windowWidth="14400" windowHeight="17480"/>
+    <workbookView xWindow="10420" yWindow="0" windowWidth="17440" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="FIS PreWork - Ruby &amp; Rails" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DateList">'FIS PreWork - Ruby &amp; Rails'!$E$5:$E$36</definedName>
+    <definedName name="DateList">'FIS PreWork - Ruby &amp; Rails'!$E$5:$E$39</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Course / Subject</t>
   </si>
@@ -97,18 +97,6 @@
     <t>Introduction to Programming</t>
   </si>
   <si>
-    <t>Javascript</t>
-  </si>
-  <si>
-    <t>Javascript Foundations</t>
-  </si>
-  <si>
-    <t>jQuery Air, First Flight</t>
-  </si>
-  <si>
-    <t>jQuery Air, Captain's Log</t>
-  </si>
-  <si>
     <t>Ruby</t>
   </si>
   <si>
@@ -169,13 +157,31 @@
   </si>
   <si>
     <t>Command Line Basics</t>
+  </si>
+  <si>
+    <t>Getting Started with Version Control</t>
+  </si>
+  <si>
+    <t>Difference between Git / Github</t>
+  </si>
+  <si>
+    <t>Git Basics and Setup</t>
+  </si>
+  <si>
+    <t>Code Academy Ruby Track</t>
+  </si>
+  <si>
+    <t>Treehouse SQL Course</t>
+  </si>
+  <si>
+    <t>ZetCode SQL Course</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +222,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,8 +309,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DCDB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -732,8 +751,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -743,8 +799,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -812,9 +870,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -851,39 +906,75 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -893,41 +984,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -935,16 +1002,13 @@
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1235,13 +1299,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E39"/>
+  <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD17"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1256,33 +1320,33 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="34" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="57" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1293,8 +1357,8 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
@@ -1303,8 +1367,8 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="13" t="s">
         <v>5</v>
       </c>
@@ -1313,44 +1377,44 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="45"/>
-      <c r="C8" s="47" t="s">
+      <c r="B8" s="56"/>
+      <c r="C8" s="58" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="38">
+        <v>39</v>
+      </c>
+      <c r="E8" s="36">
         <v>41421</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B9" s="45"/>
-      <c r="C9" s="48"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="45"/>
-      <c r="C10" s="48"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="45"/>
-      <c r="C11" s="48"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="45"/>
-      <c r="C12" s="48"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="11" t="s">
         <v>9</v>
       </c>
@@ -1359,250 +1423,270 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B13" s="45"/>
-      <c r="C13" s="49"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="60"/>
       <c r="D13" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B14" s="56"/>
+      <c r="C14" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B15" s="56"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="2:5" ht="15" thickBot="1">
+      <c r="B16" s="56"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="10">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B17" s="56"/>
+      <c r="C17" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="36">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B18" s="56"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B19" s="56"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B20" s="56"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B21" s="56"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="40">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B22" s="56"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B23" s="56"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B24" s="56"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="10">
+        <v>41427</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B25" s="5"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B26" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="37">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B27" s="46"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="38">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B28" s="46"/>
+      <c r="C28" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="37"/>
-    </row>
-    <row r="14" spans="2:5" ht="26" thickTop="1">
-      <c r="B14" s="45"/>
-      <c r="C14" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="10">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B15" s="45"/>
-      <c r="C15" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="10">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="12">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="10">
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="24">
         <v>41427</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="3.75" customHeight="1">
-      <c r="B20" s="5"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B21" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="39">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B22" s="50"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="40">
-        <v>41424</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B23" s="50"/>
-      <c r="C23" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="20" t="s">
+    <row r="30" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B30" s="46"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="24">
-        <v>41425</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B24" s="50"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B25" s="50"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="18" t="s">
+      <c r="E30" s="24"/>
+    </row>
+    <row r="31" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B31" s="46"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B26" s="50"/>
-      <c r="C26" s="53" t="s">
+      <c r="E31" s="19"/>
+    </row>
+    <row r="32" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B32" s="46"/>
+      <c r="C32" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D32" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="23"/>
+    </row>
+    <row r="33" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B33" s="46"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="37"/>
+    </row>
+    <row r="34" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B34" s="46"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="21"/>
-    </row>
-    <row r="27" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B27" s="50"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="22" t="s">
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B35" s="46"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="25">
-        <v>41427</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B28" s="50"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="18" t="s">
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B36" s="6"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="2:5" ht="26.25" customHeight="1">
+      <c r="B37" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B29" s="50"/>
-      <c r="C29" s="53" t="s">
+      <c r="D37" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="24"/>
-    </row>
-    <row r="30" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="39"/>
-    </row>
-    <row r="31" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B31" s="50"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="22" t="s">
+      <c r="E37" s="29"/>
+    </row>
+    <row r="38" spans="2:5" ht="26.25" customHeight="1" thickBot="1">
+      <c r="B38" s="42"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="25"/>
-    </row>
-    <row r="32" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B32" s="50"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="26" t="s">
+      <c r="E38" s="31"/>
+    </row>
+    <row r="39" spans="2:5" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B39" s="43"/>
+      <c r="C39" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="27"/>
-    </row>
-    <row r="33" spans="2:5" ht="3.75" customHeight="1">
-      <c r="B33" s="6"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="2:5" ht="26.25" customHeight="1">
-      <c r="B34" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="30"/>
-    </row>
-    <row r="35" spans="2:5" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B35" s="57"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="32"/>
-    </row>
-    <row r="36" spans="2:5" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B36" s="58"/>
-      <c r="C36" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="34"/>
-    </row>
-    <row r="37" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
-    <row r="38" spans="2:5" ht="18.75" customHeight="1">
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="2:5" ht="18.75" customHeight="1">
-      <c r="E39" s="8"/>
+      <c r="E39" s="33"/>
+    </row>
+    <row r="40" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
+    <row r="41" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E42" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B21:B32"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C32"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B5:B24"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C13"/>
-    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="C17:C24"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C32:C35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>

</xml_diff>

<commit_message>
Complete update on FIS Ruby-Rails prework.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -10,7 +10,7 @@
     <sheet name="FIS PreWork - Ruby &amp; Rails" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DateList">'FIS PreWork - Ruby &amp; Rails'!$E$5:$E$39</definedName>
+    <definedName name="DateList">'FIS PreWork - Ruby &amp; Rails'!$E$5:$E$42</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,12 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Course / Subject</t>
-  </si>
-  <si>
-    <t>Internet Basics</t>
   </si>
   <si>
     <t>The Web</t>
@@ -85,9 +82,6 @@
 Cmd Line</t>
   </si>
   <si>
-    <t>Programming</t>
-  </si>
-  <si>
     <t>Basics</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>Rails for Zombies 2</t>
   </si>
   <si>
-    <t>Building Facebook</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -130,14 +121,6 @@
     <t>Rails Best Practices</t>
   </si>
   <si>
-    <t>Advanced
-Topics</t>
-  </si>
-  <si>
-    <t>Best
-Practices</t>
-  </si>
-  <si>
     <t>Getting Started with Rails</t>
   </si>
   <si>
@@ -175,13 +158,34 @@
   </si>
   <si>
     <t>ZetCode SQL Course</t>
+  </si>
+  <si>
+    <t>Building Facebook I</t>
+  </si>
+  <si>
+    <t>Building Facebook II</t>
+  </si>
+  <si>
+    <t>Building Facebook III</t>
+  </si>
+  <si>
+    <t>Rails Tutorial (Michael Hartls)</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
+  <si>
+    <t>PROGRAMMING</t>
+  </si>
+  <si>
+    <t>INTERNET BASCIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +231,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -395,8 +406,36 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thick">
         <color auto="1"/>
@@ -404,21 +443,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -428,64 +456,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -784,6 +762,47 @@
       </right>
       <top/>
       <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -802,7 +821,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -816,147 +835,114 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -965,33 +951,57 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1299,13 +1309,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E42"/>
+  <dimension ref="B1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1320,211 +1330,211 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
+      <c r="B2" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="34" t="s">
-        <v>11</v>
+      <c r="E4" s="29" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="D5" s="9" t="s">
         <v>2</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>3</v>
       </c>
       <c r="E5" s="10">
         <v>41368</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="12">
         <v>41368</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="10">
         <v>41373</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="56"/>
-      <c r="C8" s="58" t="s">
-        <v>19</v>
+      <c r="B8" s="57"/>
+      <c r="C8" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="36">
+        <v>34</v>
+      </c>
+      <c r="E8" s="31">
         <v>41421</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B9" s="56"/>
-      <c r="C9" s="59"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="56"/>
-      <c r="C10" s="59"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="56"/>
-      <c r="C11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="56"/>
-      <c r="C12" s="59"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="12">
         <v>41421</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B13" s="56"/>
-      <c r="C13" s="60"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B14" s="57"/>
+      <c r="C14" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="35"/>
-    </row>
-    <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B14" s="56"/>
-      <c r="C14" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B15" s="56"/>
-      <c r="C15" s="62"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:5" ht="15" thickBot="1">
-      <c r="B16" s="56"/>
-      <c r="C16" s="63"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="10">
         <v>41421</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B17" s="56"/>
-      <c r="C17" s="58" t="s">
+      <c r="B17" s="57"/>
+      <c r="C17" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="31">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B18" s="57"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B19" s="57"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B20" s="57"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B21" s="57"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E21" s="35">
         <v>41423</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B18" s="56"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B19" s="56"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B20" s="56"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B21" s="56"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="39" t="s">
+    <row r="22" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B22" s="57"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="40">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B22" s="56"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B23" s="57"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B23" s="56"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="11" t="s">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B24" s="57"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B24" s="56"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="13" t="s">
-        <v>17</v>
       </c>
       <c r="E24" s="10">
         <v>41427</v>
@@ -1537,141 +1547,163 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="E26" s="32">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B27" s="58"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="E27" s="33">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B28" s="58"/>
+      <c r="C28" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="37">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B27" s="46"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="38">
-        <v>41424</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B28" s="46"/>
-      <c r="C28" s="49" t="s">
+      <c r="D28" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B29" s="58"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="22" t="s">
         <v>24</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B29" s="46"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="22" t="s">
-        <v>26</v>
       </c>
       <c r="E29" s="24">
         <v>41427</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B30" s="46"/>
-      <c r="C30" s="50"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="24"/>
+    </row>
+    <row r="31" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B31" s="58"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="24"/>
-    </row>
-    <row r="31" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B31" s="46"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="18" t="s">
+      <c r="E31" s="19"/>
+    </row>
+    <row r="32" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B32" s="58"/>
+      <c r="C32" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="23"/>
+    </row>
+    <row r="33" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B33" s="58"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B34" s="58"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="19"/>
-    </row>
-    <row r="32" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B32" s="46"/>
-      <c r="C32" s="49" t="s">
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B35" s="58"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B36" s="58"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="26"/>
+    </row>
+    <row r="37" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B37" s="58"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B38" s="58"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B39" s="58"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="26"/>
+    </row>
+    <row r="40" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B40" s="6"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="2:5" ht="14">
+      <c r="B41" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B33" s="46"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="37"/>
-    </row>
-    <row r="34" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B34" s="46"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="22" t="s">
+      <c r="D41" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B35" s="46"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="25" t="s">
+      <c r="E41" s="28"/>
+    </row>
+    <row r="42" spans="2:5" ht="15" thickBot="1">
+      <c r="B42" s="60"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="26"/>
-    </row>
-    <row r="36" spans="2:5" ht="3.75" customHeight="1">
-      <c r="B36" s="6"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="2:5" ht="26.25" customHeight="1">
-      <c r="B37" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="29"/>
-    </row>
-    <row r="38" spans="2:5" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B38" s="42"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="31"/>
-    </row>
-    <row r="39" spans="2:5" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B39" s="43"/>
-      <c r="C39" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="33"/>
-    </row>
-    <row r="40" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
-    <row r="41" spans="2:5" ht="18.75" customHeight="1">
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="2:5" ht="18.75" customHeight="1">
-      <c r="E42" s="8"/>
+      <c r="E42" s="54"/>
+    </row>
+    <row r="43" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
+    <row r="44" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E45" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1681,12 +1713,12 @@
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="C17:C24"/>
     <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B26:B39"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="C32:C39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>

</xml_diff>

<commit_message>
Parse out Code School Ruby Track in FIS Prework.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="0" windowWidth="17440" windowHeight="17480"/>
+    <workbookView xWindow="9080" yWindow="0" windowWidth="19720" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="FIS PreWork - Ruby &amp; Rails" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DateList">'FIS PreWork - Ruby &amp; Rails'!$E$5:$E$42</definedName>
+    <definedName name="DateList">'FIS PreWork - Ruby &amp; Rails'!$E$5:$E$45</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Course / Subject</t>
   </si>
@@ -82,9 +82,6 @@
 Cmd Line</t>
   </si>
   <si>
-    <t>Basics</t>
-  </si>
-  <si>
     <t>Try Ruby</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>Ruby Bits</t>
   </si>
   <si>
-    <t>Rails</t>
-  </si>
-  <si>
     <t>Rails for Zombies 2</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>Git Basics and Setup</t>
   </si>
   <si>
-    <t>Code Academy Ruby Track</t>
-  </si>
-  <si>
     <t>Treehouse SQL Course</t>
   </si>
   <si>
@@ -175,10 +166,22 @@
     <t>MISC</t>
   </si>
   <si>
-    <t>PROGRAMMING</t>
-  </si>
-  <si>
     <t>INTERNET BASCIS</t>
+  </si>
+  <si>
+    <t>Code School Ruby Track</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>RUBY | RAILS</t>
+  </si>
+  <si>
+    <t>Ruby Bits Pt 1</t>
+  </si>
+  <si>
+    <t>Ruby Bits Pt2</t>
   </si>
 </sst>
 </file>
@@ -327,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -807,8 +810,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,8 +851,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -883,9 +915,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -919,14 +948,68 @@
     <xf numFmtId="14" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -943,68 +1026,23 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1014,6 +1052,7 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1309,13 +1348,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E45"/>
+  <dimension ref="B1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1330,33 +1369,33 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="28" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="44" t="s">
+      <c r="B5" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1367,8 +1406,8 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="57"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1377,8 +1416,8 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="57"/>
-      <c r="C7" s="44"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1387,44 +1426,44 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="57"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="42" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="30">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B9" s="40"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B10" s="40"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="31">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B9" s="57"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="11" t="s">
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B11" s="40"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="57"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="57"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="11" t="s">
-        <v>37</v>
-      </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="57"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="11" t="s">
         <v>8</v>
       </c>
@@ -1433,34 +1472,34 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B13" s="57"/>
-      <c r="C13" s="47"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="30"/>
+        <v>36</v>
+      </c>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B14" s="57"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B15" s="57"/>
-      <c r="C15" s="49"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:5" ht="15" thickBot="1">
-      <c r="B16" s="57"/>
-      <c r="C16" s="50"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="13" t="s">
         <v>9</v>
       </c>
@@ -1469,70 +1508,70 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B17" s="57"/>
-      <c r="C17" s="45" t="s">
+      <c r="B17" s="40"/>
+      <c r="C17" s="42" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="30">
         <v>41423</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B18" s="57"/>
-      <c r="C18" s="46"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B19" s="40"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B20" s="40"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B19" s="57"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B20" s="57"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B21" s="57"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="34" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="33">
         <v>41423</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B22" s="57"/>
-      <c r="C22" s="46"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B23" s="57"/>
-      <c r="C23" s="46"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B24" s="57"/>
-      <c r="C24" s="46"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="13" t="s">
         <v>16</v>
       </c>
@@ -1547,178 +1586,204 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="25">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B27" s="52"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="62"/>
+    </row>
+    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B28" s="52"/>
+      <c r="C28" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="22">
+        <v>41427</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B29" s="52"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B30" s="52"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="19"/>
+    </row>
+    <row r="31" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B31" s="52"/>
+      <c r="C31" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="32">
+      <c r="E31" s="22">
         <v>41423</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B27" s="58"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="33">
-        <v>41424</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B28" s="58"/>
-      <c r="C28" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="55" t="s">
+    <row r="32" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B32" s="52"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="31">
+        <v>41529</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B33" s="52"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="31">
+        <v>41534</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B35" s="52"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B36" s="52"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B29" s="58"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="24">
-        <v>41427</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B30" s="58"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="24"/>
-    </row>
-    <row r="31" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B31" s="58"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="19"/>
-    </row>
-    <row r="32" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B32" s="58"/>
-      <c r="C32" s="38" t="s">
+      <c r="E36" s="25"/>
+    </row>
+    <row r="37" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B37" s="52"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="25"/>
+    </row>
+    <row r="38" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B38" s="52"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="25"/>
+    </row>
+    <row r="39" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B39" s="52"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="25"/>
+    </row>
+    <row r="40" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B40" s="52"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="25"/>
+    </row>
+    <row r="41" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B41" s="52"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="25"/>
+    </row>
+    <row r="42" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B42" s="52"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="25"/>
+    </row>
+    <row r="43" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B43" s="6"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="2:5" ht="14">
+      <c r="B44" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B33" s="58"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="32"/>
-    </row>
-    <row r="34" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B34" s="58"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="22" t="s">
+      <c r="D44" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B35" s="58"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="26"/>
-    </row>
-    <row r="36" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B36" s="58"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="26"/>
-    </row>
-    <row r="37" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B37" s="58"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B38" s="58"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B39" s="58"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" s="26"/>
-    </row>
-    <row r="40" spans="2:5" ht="3.75" customHeight="1">
-      <c r="B40" s="6"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="2:5" ht="14">
-      <c r="B41" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="51" t="s">
+      <c r="E44" s="27"/>
+    </row>
+    <row r="45" spans="2:5" ht="15" thickBot="1">
+      <c r="B45" s="49"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E41" s="28"/>
-    </row>
-    <row r="42" spans="2:5" ht="15" thickBot="1">
-      <c r="B42" s="60"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="54"/>
-    </row>
-    <row r="43" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
-    <row r="44" spans="2:5" ht="18.75" customHeight="1">
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="2:5" ht="18.75" customHeight="1">
-      <c r="E45" s="8"/>
+      <c r="E45" s="35"/>
+    </row>
+    <row r="46" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
+    <row r="47" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E48" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B26:B42"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C42"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:B24"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="C17:C24"/>
     <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B26:B39"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>

</xml_diff>

<commit_message>
Update FIS prework with complete Ruby code school track.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Course / Subject</t>
   </si>
@@ -88,27 +88,15 @@
     <t>Introduction to Programming</t>
   </si>
   <si>
-    <t>Ruby</t>
-  </si>
-  <si>
     <t>Learn to Program</t>
   </si>
   <si>
     <t>Ruby Foundations</t>
   </si>
   <si>
-    <t>Ruby Bits</t>
-  </si>
-  <si>
     <t>Rails for Zombies 2</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Testing with Rspec</t>
-  </si>
-  <si>
     <t>Rails Testing for Zombies</t>
   </si>
   <si>
@@ -163,9 +151,6 @@
     <t>Rails Tutorial (Michael Hartls)</t>
   </si>
   <si>
-    <t>MISC</t>
-  </si>
-  <si>
     <t>INTERNET BASCIS</t>
   </si>
   <si>
@@ -182,6 +167,18 @@
   </si>
   <si>
     <t>Ruby Bits Pt2</t>
+  </si>
+  <si>
+    <t>Rails 4: Zombie Outlaws</t>
+  </si>
+  <si>
+    <t>Ruby / Rails</t>
+  </si>
+  <si>
+    <t>Rails 4: Patterns</t>
+  </si>
+  <si>
+    <t>Rails Testing with Rspec</t>
   </si>
 </sst>
 </file>
@@ -244,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,12 +263,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,24 +304,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2DCDB"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -433,19 +412,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -776,70 +742,29 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color auto="1"/>
       </right>
       <top style="dashed">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
       <bottom style="double">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -852,8 +777,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -873,176 +799,152 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1053,6 +955,7 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1351,10 +1254,10 @@
   <dimension ref="B1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1369,33 +1272,33 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="41" t="s">
+      <c r="B5" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1406,8 +1309,8 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1416,8 +1319,8 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1426,44 +1329,44 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="40"/>
-      <c r="C8" s="42" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="49" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="30">
+        <v>28</v>
+      </c>
+      <c r="E8" s="28">
         <v>41421</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B9" s="40"/>
-      <c r="C9" s="43"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="40"/>
-      <c r="C10" s="43"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="40"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="40"/>
-      <c r="C12" s="43"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="11" t="s">
         <v>8</v>
       </c>
@@ -1472,34 +1375,34 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B13" s="40"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B14" s="47"/>
+      <c r="C14" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="29"/>
-    </row>
-    <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B14" s="40"/>
-      <c r="C14" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>40</v>
-      </c>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B15" s="40"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:5" ht="15" thickBot="1">
-      <c r="B16" s="40"/>
-      <c r="C16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="13" t="s">
         <v>9</v>
       </c>
@@ -1508,70 +1411,70 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B17" s="40"/>
-      <c r="C17" s="42" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="49" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="28">
         <v>41423</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B18" s="40"/>
-      <c r="C18" s="43"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E18" s="12"/>
     </row>
     <row r="19" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B19" s="40"/>
-      <c r="C19" s="43"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B20" s="40"/>
-      <c r="C20" s="43"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B21" s="40"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="32" t="s">
+      <c r="B21" s="47"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="31">
         <v>41423</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B22" s="40"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B23" s="40"/>
-      <c r="C23" s="43"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B24" s="40"/>
-      <c r="C24" s="43"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="13" t="s">
         <v>16</v>
       </c>
@@ -1586,11 +1489,11 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B26" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="59" t="s">
-        <v>49</v>
+      <c r="B26" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>44</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>20</v>
@@ -1600,170 +1503,167 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B27" s="52"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="61" t="s">
+      <c r="B27" s="35"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="34"/>
+    </row>
+    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="32" t="s">
         <v>22</v>
-      </c>
-      <c r="E27" s="62"/>
-    </row>
-    <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B28" s="52"/>
-      <c r="C28" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="58" t="s">
-        <v>23</v>
       </c>
       <c r="E28" s="22">
         <v>41427</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B29" s="52"/>
-      <c r="C29" s="56"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E29" s="23"/>
     </row>
-    <row r="30" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B30" s="52"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="18" t="s">
+    <row r="30" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B30" s="35"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B31" s="35"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="25"/>
+    </row>
+    <row r="32" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B32" s="35"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="25"/>
+    </row>
+    <row r="33" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B33" s="35"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="25"/>
+    </row>
+    <row r="34" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B34" s="35"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B35" s="35"/>
+      <c r="C35" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="22">
+        <v>41423</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B36" s="35"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="29">
+        <v>41529</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B37" s="35"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="29"/>
+    </row>
+    <row r="38" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B38" s="35"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="29">
+        <v>41534</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B39" s="35"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="23"/>
+    </row>
+    <row r="40" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B40" s="35"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="25"/>
+    </row>
+    <row r="41" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B41" s="35"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="25"/>
+    </row>
+    <row r="42" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B42" s="35"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="19"/>
-    </row>
-    <row r="31" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B31" s="52"/>
-      <c r="C31" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="22">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B32" s="52"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="17" t="s">
+      <c r="E42" s="25"/>
+    </row>
+    <row r="43" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B43" s="35"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="31">
-        <v>41529</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B33" s="52"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="31"/>
-    </row>
-    <row r="34" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B34" s="52"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="31">
-        <v>41534</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B35" s="52"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="21" t="s">
+      <c r="E43" s="25"/>
+    </row>
+    <row r="44" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B44" s="35"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="23"/>
-    </row>
-    <row r="36" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B36" s="52"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="25"/>
-    </row>
-    <row r="37" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B37" s="52"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="25"/>
-    </row>
-    <row r="38" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B38" s="52"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="25"/>
-    </row>
-    <row r="39" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B39" s="52"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="25"/>
-    </row>
-    <row r="40" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B40" s="52"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="25"/>
-    </row>
-    <row r="41" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B41" s="52"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E41" s="25"/>
-    </row>
-    <row r="42" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B42" s="52"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E42" s="25"/>
-    </row>
-    <row r="43" spans="2:5" ht="3.75" customHeight="1">
-      <c r="B43" s="6"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="2:5" ht="14">
-      <c r="B44" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="27"/>
-    </row>
-    <row r="45" spans="2:5" ht="15" thickBot="1">
-      <c r="B45" s="49"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="35"/>
-    </row>
-    <row r="46" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
+      <c r="E44" s="25"/>
+    </row>
+    <row r="45" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B45" s="6"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="3"/>
+    </row>
     <row r="47" spans="2:5" ht="18.75" customHeight="1">
       <c r="E47" s="8"/>
     </row>
@@ -1771,19 +1671,17 @@
       <c r="E48" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B26:B42"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C42"/>
-    <mergeCell ref="C26:C27"/>
+  <mergeCells count="10">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:B24"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="C17:C24"/>
     <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B26:B44"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>

</xml_diff>

<commit_message>
Complete Ruby Bits 2.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -883,6 +883,42 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -892,56 +928,20 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1254,10 +1254,10 @@
   <dimension ref="B1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1272,12 +1272,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
@@ -1295,10 +1295,10 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="40" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1309,8 +1309,8 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1319,8 +1319,8 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1329,8 +1329,8 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="47"/>
-      <c r="C8" s="49" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="41" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -1341,32 +1341,32 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B9" s="47"/>
-      <c r="C9" s="50"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="47"/>
-      <c r="C10" s="50"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="47"/>
-      <c r="C11" s="50"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="47"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="11" t="s">
         <v>8</v>
       </c>
@@ -1375,16 +1375,16 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B13" s="47"/>
-      <c r="C13" s="51"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="16" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="27"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B14" s="47"/>
-      <c r="C14" s="52" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="44" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="13" t="s">
@@ -1393,16 +1393,16 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B15" s="47"/>
-      <c r="C15" s="53"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:5" ht="15" thickBot="1">
-      <c r="B16" s="47"/>
-      <c r="C16" s="54"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="13" t="s">
         <v>9</v>
       </c>
@@ -1411,8 +1411,8 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B17" s="47"/>
-      <c r="C17" s="49" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -1423,32 +1423,32 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B18" s="47"/>
-      <c r="C18" s="50"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="12"/>
     </row>
     <row r="19" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B19" s="47"/>
-      <c r="C19" s="50"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B20" s="47"/>
-      <c r="C20" s="50"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B21" s="47"/>
-      <c r="C21" s="50"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="30" t="s">
         <v>13</v>
       </c>
@@ -1457,24 +1457,24 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B22" s="47"/>
-      <c r="C22" s="50"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B23" s="47"/>
-      <c r="C23" s="50"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B24" s="47"/>
-      <c r="C24" s="50"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="13" t="s">
         <v>16</v>
       </c>
@@ -1489,10 +1489,10 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="53" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="24" t="s">
@@ -1503,16 +1503,16 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B27" s="35"/>
-      <c r="C27" s="42"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="54"/>
       <c r="D27" s="33" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="34"/>
     </row>
     <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B28" s="35"/>
-      <c r="C28" s="36" t="s">
+      <c r="B28" s="47"/>
+      <c r="C28" s="48" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="32" t="s">
@@ -1523,56 +1523,56 @@
       </c>
     </row>
     <row r="29" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="21" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="23"/>
     </row>
     <row r="30" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B30" s="35"/>
-      <c r="C30" s="40"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="24" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="40"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="24" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="25"/>
     </row>
     <row r="32" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B32" s="35"/>
-      <c r="C32" s="40"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="24" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="25"/>
     </row>
     <row r="33" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B33" s="35"/>
-      <c r="C33" s="40"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="50"/>
       <c r="D33" s="24" t="s">
         <v>40</v>
       </c>
       <c r="E33" s="25"/>
     </row>
     <row r="34" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B34" s="35"/>
-      <c r="C34" s="38"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B35" s="35"/>
-      <c r="C35" s="36" t="s">
+      <c r="B35" s="47"/>
+      <c r="C35" s="48" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="20" t="s">
@@ -1583,8 +1583,8 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B36" s="35"/>
-      <c r="C36" s="39"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="52"/>
       <c r="D36" s="17" t="s">
         <v>46</v>
       </c>
@@ -1593,16 +1593,18 @@
       </c>
     </row>
     <row r="37" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B37" s="35"/>
-      <c r="C37" s="39"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="52"/>
       <c r="D37" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="E37" s="29">
+        <v>41532</v>
+      </c>
     </row>
     <row r="38" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B38" s="35"/>
-      <c r="C38" s="39"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="52"/>
       <c r="D38" s="17" t="s">
         <v>27</v>
       </c>
@@ -1611,48 +1613,48 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B39" s="35"/>
-      <c r="C39" s="37"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="21" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="23"/>
     </row>
     <row r="40" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B40" s="35"/>
-      <c r="C40" s="40"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="24" t="s">
         <v>48</v>
       </c>
       <c r="E40" s="25"/>
     </row>
     <row r="41" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B41" s="35"/>
-      <c r="C41" s="40"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="24" t="s">
         <v>50</v>
       </c>
       <c r="E41" s="25"/>
     </row>
     <row r="42" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B42" s="35"/>
-      <c r="C42" s="40"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E42" s="25"/>
     </row>
     <row r="43" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B43" s="35"/>
-      <c r="C43" s="40"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="24" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="25"/>
     </row>
     <row r="44" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B44" s="35"/>
-      <c r="C44" s="40"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="24" t="s">
         <v>25</v>
       </c>
@@ -1672,16 +1674,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B26:B44"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:B24"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="C17:C24"/>
     <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B26:B44"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="C35:C44"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>

</xml_diff>

<commit_message>
Update FIS Prework with updated coursework.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="9080" yWindow="0" windowWidth="19720" windowHeight="17480"/>
@@ -883,6 +883,30 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -918,30 +942,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1257,7 +1257,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1272,12 +1272,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
@@ -1295,10 +1295,10 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="48" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1309,8 +1309,8 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1319,8 +1319,8 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1329,8 +1329,8 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="39"/>
-      <c r="C8" s="41" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="49" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -1341,32 +1341,32 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B9" s="39"/>
-      <c r="C9" s="42"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="39"/>
-      <c r="C10" s="42"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="39"/>
-      <c r="C11" s="42"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="39"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="11" t="s">
         <v>8</v>
       </c>
@@ -1375,16 +1375,16 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B13" s="39"/>
-      <c r="C13" s="43"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="16" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="27"/>
     </row>
     <row r="14" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B14" s="39"/>
-      <c r="C14" s="44" t="s">
+      <c r="B14" s="47"/>
+      <c r="C14" s="52" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="13" t="s">
@@ -1393,16 +1393,16 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B15" s="39"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:5" ht="15" thickBot="1">
-      <c r="B16" s="39"/>
-      <c r="C16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="13" t="s">
         <v>9</v>
       </c>
@@ -1411,8 +1411,8 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B17" s="39"/>
-      <c r="C17" s="41" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="49" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -1423,32 +1423,32 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B18" s="39"/>
-      <c r="C18" s="42"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="12"/>
     </row>
     <row r="19" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B19" s="39"/>
-      <c r="C19" s="42"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="12"/>
     </row>
     <row r="20" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B20" s="39"/>
-      <c r="C20" s="42"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B21" s="39"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="30" t="s">
         <v>13</v>
       </c>
@@ -1457,24 +1457,24 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B22" s="39"/>
-      <c r="C22" s="42"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B23" s="39"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B24" s="39"/>
-      <c r="C24" s="42"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="13" t="s">
         <v>16</v>
       </c>
@@ -1489,10 +1489,10 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="53" t="s">
+      <c r="C26" s="41" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="24" t="s">
@@ -1503,16 +1503,16 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B27" s="47"/>
-      <c r="C27" s="54"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="33" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="34"/>
     </row>
     <row r="28" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B28" s="47"/>
-      <c r="C28" s="48" t="s">
+      <c r="B28" s="35"/>
+      <c r="C28" s="36" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="32" t="s">
@@ -1523,56 +1523,56 @@
       </c>
     </row>
     <row r="29" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B29" s="47"/>
-      <c r="C29" s="49"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="23"/>
     </row>
     <row r="30" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B30" s="47"/>
-      <c r="C30" s="50"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="24" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B31" s="47"/>
-      <c r="C31" s="50"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="24" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="25"/>
     </row>
     <row r="32" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B32" s="47"/>
-      <c r="C32" s="50"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="38"/>
       <c r="D32" s="24" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="25"/>
     </row>
     <row r="33" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B33" s="47"/>
-      <c r="C33" s="50"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="38"/>
       <c r="D33" s="24" t="s">
         <v>40</v>
       </c>
       <c r="E33" s="25"/>
     </row>
     <row r="34" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B34" s="47"/>
-      <c r="C34" s="51"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="39"/>
       <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B35" s="47"/>
-      <c r="C35" s="48" t="s">
+      <c r="B35" s="35"/>
+      <c r="C35" s="36" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="20" t="s">
@@ -1583,8 +1583,8 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B36" s="47"/>
-      <c r="C36" s="52"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="40"/>
       <c r="D36" s="17" t="s">
         <v>46</v>
       </c>
@@ -1593,8 +1593,8 @@
       </c>
     </row>
     <row r="37" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B37" s="47"/>
-      <c r="C37" s="52"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="17" t="s">
         <v>47</v>
       </c>
@@ -1603,8 +1603,8 @@
       </c>
     </row>
     <row r="38" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B38" s="47"/>
-      <c r="C38" s="52"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="40"/>
       <c r="D38" s="17" t="s">
         <v>27</v>
       </c>
@@ -1613,52 +1613,54 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B39" s="47"/>
-      <c r="C39" s="49"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="21" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="23"/>
     </row>
     <row r="40" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B40" s="47"/>
-      <c r="C40" s="50"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="38"/>
       <c r="D40" s="24" t="s">
         <v>48</v>
       </c>
       <c r="E40" s="25"/>
     </row>
     <row r="41" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B41" s="47"/>
-      <c r="C41" s="50"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="38"/>
       <c r="D41" s="24" t="s">
         <v>50</v>
       </c>
       <c r="E41" s="25"/>
     </row>
     <row r="42" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B42" s="47"/>
-      <c r="C42" s="50"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E42" s="25"/>
     </row>
     <row r="43" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B43" s="47"/>
-      <c r="C43" s="50"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="24" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="25"/>
     </row>
     <row r="44" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B44" s="47"/>
-      <c r="C44" s="50"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="25"/>
+      <c r="E44" s="25">
+        <v>41584</v>
+      </c>
     </row>
     <row r="45" spans="2:5" ht="3.75" customHeight="1">
       <c r="B45" s="6"/>

</xml_diff>

<commit_message>
Update XLS with Code School course completions.
</commit_message>
<xml_diff>
--- a/FIS_Prework_Ruby-Rails.xlsx
+++ b/FIS_Prework_Ruby-Rails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="0" windowWidth="19720" windowHeight="17480"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="FIS PreWork - Ruby &amp; Rails" sheetId="1" r:id="rId1"/>
@@ -1257,7 +1257,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1618,7 +1618,9 @@
       <c r="D39" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E39" s="23"/>
+      <c r="E39" s="23">
+        <v>41545</v>
+      </c>
     </row>
     <row r="40" spans="2:5" ht="18.75" customHeight="1">
       <c r="B40" s="35"/>
@@ -1642,7 +1644,9 @@
       <c r="D42" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="25"/>
+      <c r="E42" s="25">
+        <v>41546</v>
+      </c>
     </row>
     <row r="43" spans="2:5" ht="18.75" customHeight="1">
       <c r="B43" s="35"/>
@@ -1650,7 +1654,9 @@
       <c r="D43" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E43" s="25"/>
+      <c r="E43" s="25">
+        <v>41546</v>
+      </c>
     </row>
     <row r="44" spans="2:5" ht="18.75" customHeight="1">
       <c r="B44" s="35"/>

</xml_diff>